<commit_message>
reorganized files , Read Write Excel Files
</commit_message>
<xml_diff>
--- a/3 - Pandas, Data Visualization/Pandas/2 - Read Write Excel  CSV File/newExcel.xlsx
+++ b/3 - Pandas, Data Visualization/Pandas/2 - Read Write Excel  CSV File/newExcel.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="C2:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -433,148 +433,133 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="B1" s="1" t="inlineStr">
+    <row r="2">
+      <c r="C2" s="1" t="inlineStr">
         <is>
           <t>tickers</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D2" s="1" t="inlineStr">
         <is>
           <t>eps</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E2" s="1" t="inlineStr">
         <is>
           <t>revenue</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F2" s="1" t="inlineStr">
         <is>
           <t>price</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G2" s="1" t="inlineStr">
         <is>
           <t>people</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>GOOGL</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>27.82</v>
-      </c>
-      <c r="D2" t="n">
-        <v>87</v>
-      </c>
-      <c r="E2" t="n">
-        <v>845</v>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>larry page</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>WMT</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>4.61</v>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>GOOGL</t>
+        </is>
       </c>
       <c r="D3" t="n">
-        <v>484</v>
+        <v>27.82</v>
       </c>
       <c r="E3" t="n">
-        <v>65</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>efekan alipasha</t>
+        <v>87</v>
+      </c>
+      <c r="F3" t="n">
+        <v>845</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>larry page</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>MSFT</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>-1</v>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>WMT</t>
+        </is>
       </c>
       <c r="D4" t="n">
-        <v>85</v>
+        <v>4.61</v>
       </c>
       <c r="E4" t="n">
-        <v>64</v>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>bill gates</t>
+        <v>484</v>
+      </c>
+      <c r="F4" t="n">
+        <v>65</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>efekan alipasha</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>RIL</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr"/>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>MSFT</t>
+        </is>
+      </c>
       <c r="D5" t="n">
-        <v>50</v>
+        <v>-1</v>
       </c>
       <c r="E5" t="n">
-        <v>1023</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>mukesh ambani</t>
+        <v>85</v>
+      </c>
+      <c r="F5" t="n">
+        <v>64</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>bill gates</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="inlineStr">
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>RIL</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="n">
+        <v>50</v>
+      </c>
+      <c r="F6" t="n">
+        <v>1023</v>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>mukesh ambani</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="C7" t="inlineStr">
         <is>
           <t>TATA</t>
         </is>
       </c>
-      <c r="C6" t="n">
+      <c r="D7" t="n">
         <v>5.6</v>
       </c>
-      <c r="D6" t="n">
+      <c r="E7" t="n">
         <v>-1</v>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="F7" t="inlineStr">
         <is>
           <t>n.a.</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="G7" t="inlineStr">
         <is>
           <t>ratan tata</t>
         </is>

</xml_diff>